<commit_message>
fix handle fetch error response and  account-excel-export
</commit_message>
<xml_diff>
--- a/banking-report-service/src/main/resources/template/account.xlsx
+++ b/banking-report-service/src/main/resources/template/account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nvs/Downloads/Work/KLB/microservices-core-banking/banking-report-service/src/main/resources/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB52E217-A211-8C43-822A-4877CFB33A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4769EB9D-42A1-E841-9182-16050FE0C8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{E2CCA71D-B452-3C4E-A0F0-45F48612AB07}"/>
   </bookViews>
@@ -80,6 +80,39 @@
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{624EDF0A-35DF-E548-9D5D-2E5FD51DCBA4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nguyễn Văn Sĩ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:area(lastCell="F18")</t>
         </r>
       </text>
     </comment>
@@ -773,7 +806,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>